<commit_message>
Fixes on the market price generator function
</commit_message>
<xml_diff>
--- a/data/raw/intraday_price_profile.xlsx
+++ b/data/raw/intraday_price_profile.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19FE42AB-6FC7-4A91-A0CE-42C66A53806B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1365" windowWidth="19200" windowHeight="8835"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Price" sheetId="1" r:id="rId1"/>
@@ -19,15 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="3">
   <si>
     <t>month</t>
   </si>
   <si>
     <t>day</t>
-  </si>
-  <si>
-    <t>ENDE</t>
   </si>
   <si>
     <t>2-4</t>
@@ -36,7 +34,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -349,16 +347,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CU61"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:CT61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="BZ1" workbookViewId="0">
+      <selection activeCell="CU1" sqref="CU1:CU1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -654,7 +652,7 @@
         <v>0.98958333333333193</v>
       </c>
     </row>
-    <row r="2" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -949,16 +947,13 @@
       <c r="CT2">
         <v>46.390596710594792</v>
       </c>
-      <c r="CU2" t="s">
-        <v>2</v>
-      </c>
     </row>
-    <row r="3" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C3">
         <v>110.44896642686982</v>
@@ -1248,11 +1243,8 @@
       <c r="CT3">
         <v>57.814994795538112</v>
       </c>
-      <c r="CU3" t="s">
-        <v>2</v>
-      </c>
     </row>
-    <row r="4" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1547,11 +1539,8 @@
       <c r="CT4">
         <v>54.013844560277555</v>
       </c>
-      <c r="CU4" t="s">
-        <v>2</v>
-      </c>
     </row>
-    <row r="5" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1846,11 +1835,8 @@
       <c r="CT5">
         <v>48.480054973976486</v>
       </c>
-      <c r="CU5" t="s">
-        <v>2</v>
-      </c>
     </row>
-    <row r="6" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1</v>
       </c>
@@ -2145,11 +2131,8 @@
       <c r="CT6">
         <v>38.907331006399794</v>
       </c>
-      <c r="CU6" t="s">
-        <v>2</v>
-      </c>
     </row>
-    <row r="7" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2</v>
       </c>
@@ -2444,16 +2427,13 @@
       <c r="CT7">
         <v>47.718372308941653</v>
       </c>
-      <c r="CU7" t="s">
-        <v>2</v>
-      </c>
     </row>
-    <row r="8" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C8">
         <v>97.722572553785042</v>
@@ -2743,11 +2723,8 @@
       <c r="CT8">
         <v>49.944902818210416</v>
       </c>
-      <c r="CU8" t="s">
-        <v>2</v>
-      </c>
     </row>
-    <row r="9" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2</v>
       </c>
@@ -3042,11 +3019,8 @@
       <c r="CT9">
         <v>44.394374261547128</v>
       </c>
-      <c r="CU9" t="s">
-        <v>2</v>
-      </c>
     </row>
-    <row r="10" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2</v>
       </c>
@@ -3341,11 +3315,8 @@
       <c r="CT10">
         <v>46.078269574974371</v>
       </c>
-      <c r="CU10" t="s">
-        <v>2</v>
-      </c>
     </row>
-    <row r="11" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2</v>
       </c>
@@ -3640,11 +3611,8 @@
       <c r="CT11">
         <v>19.205165088962428</v>
       </c>
-      <c r="CU11" t="s">
-        <v>2</v>
-      </c>
     </row>
-    <row r="12" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>3</v>
       </c>
@@ -3939,16 +3907,13 @@
       <c r="CT12">
         <v>56.155956658200544</v>
       </c>
-      <c r="CU12" t="s">
-        <v>2</v>
-      </c>
     </row>
-    <row r="13" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>3</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C13">
         <v>85.91887262564326</v>
@@ -4238,11 +4203,8 @@
       <c r="CT13">
         <v>59.759623322740794</v>
       </c>
-      <c r="CU13" t="s">
-        <v>2</v>
-      </c>
     </row>
-    <row r="14" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>3</v>
       </c>
@@ -4537,11 +4499,8 @@
       <c r="CT14">
         <v>61.624250011291728</v>
       </c>
-      <c r="CU14" t="s">
-        <v>2</v>
-      </c>
     </row>
-    <row r="15" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>3</v>
       </c>
@@ -4836,11 +4795,8 @@
       <c r="CT15">
         <v>51.616280401881262</v>
       </c>
-      <c r="CU15" t="s">
-        <v>2</v>
-      </c>
     </row>
-    <row r="16" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>3</v>
       </c>
@@ -5135,11 +5091,8 @@
       <c r="CT16">
         <v>44.382213068373119</v>
       </c>
-      <c r="CU16" t="s">
-        <v>2</v>
-      </c>
     </row>
-    <row r="17" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>4</v>
       </c>
@@ -5434,16 +5387,13 @@
       <c r="CT17">
         <v>48.761303504818912</v>
       </c>
-      <c r="CU17" t="s">
-        <v>2</v>
-      </c>
     </row>
-    <row r="18" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>4</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C18">
         <v>100.20714618807051</v>
@@ -5733,11 +5683,8 @@
       <c r="CT18">
         <v>63.079711905052264</v>
       </c>
-      <c r="CU18" t="s">
-        <v>2</v>
-      </c>
     </row>
-    <row r="19" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>4</v>
       </c>
@@ -6032,11 +5979,8 @@
       <c r="CT19">
         <v>57.841185134918135</v>
       </c>
-      <c r="CU19" t="s">
-        <v>2</v>
-      </c>
     </row>
-    <row r="20" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>4</v>
       </c>
@@ -6331,11 +6275,8 @@
       <c r="CT20">
         <v>66.427490576187381</v>
       </c>
-      <c r="CU20" t="s">
-        <v>2</v>
-      </c>
     </row>
-    <row r="21" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>4</v>
       </c>
@@ -6630,11 +6571,8 @@
       <c r="CT21">
         <v>45.128555847147368</v>
       </c>
-      <c r="CU21" t="s">
-        <v>2</v>
-      </c>
     </row>
-    <row r="22" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>5</v>
       </c>
@@ -6929,16 +6867,13 @@
       <c r="CT22">
         <v>61.350706919650477</v>
       </c>
-      <c r="CU22" t="s">
-        <v>2</v>
-      </c>
     </row>
-    <row r="23" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>5</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C23">
         <v>99.365519757246062</v>
@@ -7228,11 +7163,8 @@
       <c r="CT23">
         <v>69.285197435732769</v>
       </c>
-      <c r="CU23" t="s">
-        <v>2</v>
-      </c>
     </row>
-    <row r="24" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>5</v>
       </c>
@@ -7527,11 +7459,8 @@
       <c r="CT24">
         <v>68.192355219058896</v>
       </c>
-      <c r="CU24" t="s">
-        <v>2</v>
-      </c>
     </row>
-    <row r="25" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>5</v>
       </c>
@@ -7826,11 +7755,8 @@
       <c r="CT25">
         <v>66.854958989013753</v>
       </c>
-      <c r="CU25" t="s">
-        <v>2</v>
-      </c>
     </row>
-    <row r="26" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>5</v>
       </c>
@@ -8125,11 +8051,8 @@
       <c r="CT26">
         <v>50.957353677150032</v>
       </c>
-      <c r="CU26" t="s">
-        <v>2</v>
-      </c>
     </row>
-    <row r="27" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>6</v>
       </c>
@@ -8424,16 +8347,13 @@
       <c r="CT27">
         <v>80.407481149711174</v>
       </c>
-      <c r="CU27" t="s">
-        <v>2</v>
-      </c>
     </row>
-    <row r="28" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>6</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C28">
         <v>114.40357313384028</v>
@@ -8723,11 +8643,8 @@
       <c r="CT28">
         <v>75.457103388640931</v>
       </c>
-      <c r="CU28" t="s">
-        <v>2</v>
-      </c>
     </row>
-    <row r="29" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>6</v>
       </c>
@@ -9022,11 +8939,8 @@
       <c r="CT29">
         <v>83.96604866650172</v>
       </c>
-      <c r="CU29" t="s">
-        <v>2</v>
-      </c>
     </row>
-    <row r="30" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>6</v>
       </c>
@@ -9321,11 +9235,8 @@
       <c r="CT30">
         <v>77.917401202148412</v>
       </c>
-      <c r="CU30" t="s">
-        <v>2</v>
-      </c>
     </row>
-    <row r="31" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>6</v>
       </c>
@@ -9620,11 +9531,8 @@
       <c r="CT31">
         <v>76.558675423010214</v>
       </c>
-      <c r="CU31" t="s">
-        <v>2</v>
-      </c>
     </row>
-    <row r="32" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>7</v>
       </c>
@@ -9919,16 +9827,13 @@
       <c r="CT32">
         <v>72.678484256581669</v>
       </c>
-      <c r="CU32" t="s">
-        <v>2</v>
-      </c>
     </row>
-    <row r="33" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>7</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C33">
         <v>113.20083561357812</v>
@@ -10218,11 +10123,8 @@
       <c r="CT33">
         <v>79.498443171571992</v>
       </c>
-      <c r="CU33" t="s">
-        <v>2</v>
-      </c>
     </row>
-    <row r="34" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>7</v>
       </c>
@@ -10517,11 +10419,8 @@
       <c r="CT34">
         <v>73.864340182337273</v>
       </c>
-      <c r="CU34" t="s">
-        <v>2</v>
-      </c>
     </row>
-    <row r="35" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>7</v>
       </c>
@@ -10816,11 +10715,8 @@
       <c r="CT35">
         <v>73.774688008774575</v>
       </c>
-      <c r="CU35" t="s">
-        <v>2</v>
-      </c>
     </row>
-    <row r="36" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>7</v>
       </c>
@@ -11115,11 +11011,8 @@
       <c r="CT36">
         <v>64.843839357510518</v>
       </c>
-      <c r="CU36" t="s">
-        <v>2</v>
-      </c>
     </row>
-    <row r="37" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>8</v>
       </c>
@@ -11414,16 +11307,13 @@
       <c r="CT37">
         <v>72.179050551340325</v>
       </c>
-      <c r="CU37" t="s">
-        <v>2</v>
-      </c>
     </row>
-    <row r="38" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>8</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C38">
         <v>102.53563732992703</v>
@@ -11713,11 +11603,8 @@
       <c r="CT38">
         <v>63.607116365724046</v>
       </c>
-      <c r="CU38" t="s">
-        <v>2</v>
-      </c>
     </row>
-    <row r="39" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>8</v>
       </c>
@@ -12012,11 +11899,8 @@
       <c r="CT39">
         <v>66.697388341001584</v>
       </c>
-      <c r="CU39" t="s">
-        <v>2</v>
-      </c>
     </row>
-    <row r="40" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>8</v>
       </c>
@@ -12311,11 +12195,8 @@
       <c r="CT40">
         <v>70.166399403971027</v>
       </c>
-      <c r="CU40" t="s">
-        <v>2</v>
-      </c>
     </row>
-    <row r="41" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>8</v>
       </c>
@@ -12610,11 +12491,8 @@
       <c r="CT41">
         <v>59.783934282080907</v>
       </c>
-      <c r="CU41" t="s">
-        <v>2</v>
-      </c>
     </row>
-    <row r="42" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>9</v>
       </c>
@@ -12909,16 +12787,13 @@
       <c r="CT42">
         <v>52.298100098152176</v>
       </c>
-      <c r="CU42" t="s">
-        <v>2</v>
-      </c>
     </row>
-    <row r="43" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>9</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C43">
         <v>110.66606819560054</v>
@@ -13208,11 +13083,8 @@
       <c r="CT43">
         <v>44.076457624791885</v>
       </c>
-      <c r="CU43" t="s">
-        <v>2</v>
-      </c>
     </row>
-    <row r="44" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>9</v>
       </c>
@@ -13507,11 +13379,8 @@
       <c r="CT44">
         <v>50.531658738425541</v>
       </c>
-      <c r="CU44" t="s">
-        <v>2</v>
-      </c>
     </row>
-    <row r="45" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>9</v>
       </c>
@@ -13806,11 +13675,8 @@
       <c r="CT45">
         <v>48.793409501490423</v>
       </c>
-      <c r="CU45" t="s">
-        <v>2</v>
-      </c>
     </row>
-    <row r="46" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>9</v>
       </c>
@@ -14105,11 +13971,8 @@
       <c r="CT46">
         <v>30.900095436525799</v>
       </c>
-      <c r="CU46" t="s">
-        <v>2</v>
-      </c>
     </row>
-    <row r="47" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>10</v>
       </c>
@@ -14404,16 +14267,13 @@
       <c r="CT47">
         <v>57.672643940962566</v>
       </c>
-      <c r="CU47" t="s">
-        <v>2</v>
-      </c>
     </row>
-    <row r="48" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>10</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C48">
         <v>133.6668680242297</v>
@@ -14703,11 +14563,8 @@
       <c r="CT48">
         <v>68.405483200441736</v>
       </c>
-      <c r="CU48" t="s">
-        <v>2</v>
-      </c>
     </row>
-    <row r="49" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>10</v>
       </c>
@@ -15002,11 +14859,8 @@
       <c r="CT49">
         <v>61.495826024605691</v>
       </c>
-      <c r="CU49" t="s">
-        <v>2</v>
-      </c>
     </row>
-    <row r="50" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>10</v>
       </c>
@@ -15301,11 +15155,8 @@
       <c r="CT50">
         <v>67.685862182872341</v>
       </c>
-      <c r="CU50" t="s">
-        <v>2</v>
-      </c>
     </row>
-    <row r="51" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>10</v>
       </c>
@@ -15600,11 +15451,8 @@
       <c r="CT51">
         <v>58.476211171940861</v>
       </c>
-      <c r="CU51" t="s">
-        <v>2</v>
-      </c>
     </row>
-    <row r="52" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>11</v>
       </c>
@@ -15899,16 +15747,13 @@
       <c r="CT52">
         <v>22.197658018724749</v>
       </c>
-      <c r="CU52" t="s">
-        <v>2</v>
-      </c>
     </row>
-    <row r="53" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>11</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C53">
         <v>117.51345170286159</v>
@@ -16198,11 +16043,8 @@
       <c r="CT53">
         <v>37.523715435556248</v>
       </c>
-      <c r="CU53" t="s">
-        <v>2</v>
-      </c>
     </row>
-    <row r="54" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>11</v>
       </c>
@@ -16497,11 +16339,8 @@
       <c r="CT54">
         <v>41.80200766630292</v>
       </c>
-      <c r="CU54" t="s">
-        <v>2</v>
-      </c>
     </row>
-    <row r="55" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>11</v>
       </c>
@@ -16796,11 +16635,8 @@
       <c r="CT55">
         <v>29.671077883940484</v>
       </c>
-      <c r="CU55" t="s">
-        <v>2</v>
-      </c>
     </row>
-    <row r="56" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>11</v>
       </c>
@@ -17095,11 +16931,8 @@
       <c r="CT56">
         <v>9.6112511635825193</v>
       </c>
-      <c r="CU56" t="s">
-        <v>2</v>
-      </c>
     </row>
-    <row r="57" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>12</v>
       </c>
@@ -17394,16 +17227,13 @@
       <c r="CT57">
         <v>31.918832670041724</v>
       </c>
-      <c r="CU57" t="s">
-        <v>2</v>
-      </c>
     </row>
-    <row r="58" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>12</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C58">
         <v>104.86332208861133</v>
@@ -17693,11 +17523,8 @@
       <c r="CT58">
         <v>28.294087360029156</v>
       </c>
-      <c r="CU58" t="s">
-        <v>2</v>
-      </c>
     </row>
-    <row r="59" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>12</v>
       </c>
@@ -17992,11 +17819,8 @@
       <c r="CT59">
         <v>57.09852756619663</v>
       </c>
-      <c r="CU59" t="s">
-        <v>2</v>
-      </c>
     </row>
-    <row r="60" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>12</v>
       </c>
@@ -18291,11 +18115,8 @@
       <c r="CT60">
         <v>57.734898997365605</v>
       </c>
-      <c r="CU60" t="s">
-        <v>2</v>
-      </c>
     </row>
-    <row r="61" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>12</v>
       </c>
@@ -18589,9 +18410,6 @@
       </c>
       <c r="CT61">
         <v>39.278476327922419</v>
-      </c>
-      <c r="CU61" t="s">
-        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>